<commit_message>
Added the first prototyp of the nlp-pipeline.
</commit_message>
<xml_diff>
--- a/Database/time_memory_analysis.xlsx
+++ b/Database/time_memory_analysis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\ATS\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\didid\GitHub-Respository\AutomaticTextSummarization\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1710CC40-A677-40A2-A353-FBF45A09D657}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAC62D5-9C1E-4A85-83CA-ADE88B123204}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4B6C81A6-BA5B-4316-85AC-677727BB3B14}"/>
   </bookViews>
@@ -616,7 +616,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="2">
-        <v>200000</v>
+        <v>20000</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>7</v>
@@ -644,18 +644,18 @@
       </c>
       <c r="E3" s="4">
         <f>D3*E2</f>
-        <v>300000</v>
+        <v>30000</v>
       </c>
       <c r="F3" s="7">
         <f>E3/3600</f>
-        <v>83.333333333333329</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="G3" s="16" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="3">
         <f>F3*25/24</f>
-        <v>86.805555555555543</v>
+        <v>8.6805555555555554</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>6</v>
@@ -674,18 +674,18 @@
       </c>
       <c r="E4" s="6">
         <f>D4*E2</f>
-        <v>950</v>
+        <v>95</v>
       </c>
       <c r="F4" s="8">
         <f>E4/1000</f>
-        <v>0.95</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="G4" s="17" t="s">
         <v>5</v>
       </c>
       <c r="H4" s="5">
         <f>F4*25</f>
-        <v>23.75</v>
+        <v>2.375</v>
       </c>
       <c r="I4" s="6" t="s">
         <v>2</v>

</xml_diff>